<commit_message>
Gabungkan dengan commit dari remote
</commit_message>
<xml_diff>
--- a/kamusbakutidakbakufix.xlsx
+++ b/kamusbakutidakbakufix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\Skripsi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E3009257-55B3-4A26-8B27-7B09F31F9672}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24C6A5E9-4E3E-4B2B-9C1A-156AB9BBE362}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10308" uniqueCount="5257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10330" uniqueCount="5266">
   <si>
     <t>malming</t>
   </si>
@@ -15791,6 +15791,33 @@
   </si>
   <si>
     <t xml:space="preserve">seperti </t>
+  </si>
+  <si>
+    <t>bukan</t>
+  </si>
+  <si>
+    <t>sebaiknya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sebaik </t>
+  </si>
+  <si>
+    <t>sebaik-baiknya</t>
+  </si>
+  <si>
+    <t>sangat</t>
+  </si>
+  <si>
+    <t>sekali</t>
+  </si>
+  <si>
+    <t>sekali-kali</t>
+  </si>
+  <si>
+    <t>amatlah</t>
+  </si>
+  <si>
+    <t>sangatlah</t>
   </si>
 </sst>
 </file>
@@ -16169,10 +16196,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5155"/>
+  <dimension ref="A1:B5166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="A1785" sqref="A1785"/>
+    <sheetView tabSelected="1" topLeftCell="A5157" workbookViewId="0">
+      <selection activeCell="B5163" sqref="B5163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -57412,6 +57439,94 @@
         <v>5152</v>
       </c>
     </row>
+    <row r="5156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5156" t="s">
+        <v>5172</v>
+      </c>
+      <c r="B5156" t="s">
+        <v>5172</v>
+      </c>
+    </row>
+    <row r="5157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5157" t="s">
+        <v>5257</v>
+      </c>
+      <c r="B5157" t="s">
+        <v>5257</v>
+      </c>
+    </row>
+    <row r="5158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5158" t="s">
+        <v>5258</v>
+      </c>
+      <c r="B5158" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="5159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5159" t="s">
+        <v>5259</v>
+      </c>
+      <c r="B5159" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="5160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5160" t="s">
+        <v>5260</v>
+      </c>
+      <c r="B5160" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="5161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5161" t="s">
+        <v>5261</v>
+      </c>
+      <c r="B5161" t="s">
+        <v>5261</v>
+      </c>
+    </row>
+    <row r="5162" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5162" t="s">
+        <v>2131</v>
+      </c>
+      <c r="B5162" t="s">
+        <v>2131</v>
+      </c>
+    </row>
+    <row r="5163" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5163" t="s">
+        <v>5262</v>
+      </c>
+      <c r="B5163" t="s">
+        <v>5262</v>
+      </c>
+    </row>
+    <row r="5164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5164" t="s">
+        <v>5263</v>
+      </c>
+      <c r="B5164" t="s">
+        <v>5263</v>
+      </c>
+    </row>
+    <row r="5165" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5165" t="s">
+        <v>5264</v>
+      </c>
+      <c r="B5165" t="s">
+        <v>2131</v>
+      </c>
+    </row>
+    <row r="5166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5166" t="s">
+        <v>5265</v>
+      </c>
+      <c r="B5166" t="s">
+        <v>5261</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>